<commit_message>
FIx: remove sensitive file and clean commit
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28813"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6848B7AE-DD15-42EA-A319-CCEFFFE1C380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CD1405-C92D-2949-8B48-CDCD63280991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28560" windowHeight="13905" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="22040" windowHeight="19500" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,18 +437,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F274FABB-DF5C-4F9E-B98F-F8DC866DADF5}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,9 +459,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>12345</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -470,8 +470,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="E4" s="1"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>